<commit_message>
Added new example notebook
"Unwrapped" version of code in a notebook and an example excel sheet for
a two-state model. Good sandbox of sorts to rapidly test the
implmentation of new transiton probability functions
</commit_message>
<xml_diff>
--- a/model_specifications/test_parameters_td.xlsx
+++ b/model_specifications/test_parameters_td.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A06E2FE-EAB2-447C-BF9E-CAB0ADABD819}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="702" yWindow="702" windowWidth="14400" windowHeight="7374" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>start_state</t>
   </si>
@@ -118,13 +119,16 @@
     <t>residual</t>
   </si>
   <si>
-    <t>time_dependent</t>
+    <t>time_dependent_gompertz</t>
+  </si>
+  <si>
+    <t>static</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -435,23 +439,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.83984375" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.15625" customWidth="1"/>
+    <col min="4" max="4" width="18.41796875" customWidth="1"/>
+    <col min="5" max="5" width="12.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -479,7 +483,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -490,13 +494,13 @@
         <v>31</v>
       </c>
       <c r="D3">
-        <v>0.50572799999999996</v>
+        <v>-1.3624080000000001</v>
       </c>
       <c r="E3">
-        <v>0.231929</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-0.33633940000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -516,50 +520,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="2" width="16.41796875" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="6" max="6" width="15.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
         <v>300</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0</v>
       </c>
     </row>
@@ -569,49 +582,58 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="2" width="12.41796875" customWidth="1"/>
+    <col min="4" max="4" width="16.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
         <v>0.85</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0</v>
       </c>
     </row>
@@ -621,20 +643,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.578125" customWidth="1"/>
+    <col min="2" max="2" width="11.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -642,7 +664,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -650,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -658,7 +680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -666,7 +688,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -680,20 +702,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.26171875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -701,7 +723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -709,7 +731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -717,7 +739,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -725,7 +747,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -733,7 +755,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -741,7 +763,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -749,7 +771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>21</v>
       </c>

</xml_diff>